<commit_message>
Co-authored-by: Chokiwangchuk12180005 <Chokiwangchuk12180005@users.noreply.github.com> Co-authored-by: JarnaJee <JarnaJee@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/public/sample/student.xlsx
+++ b/public/sample/student.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="14295" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>student_code</t>
   </si>
@@ -57,6 +60,9 @@
     <t>gurdian_name</t>
   </si>
   <si>
+    <t>gurdian_contact</t>
+  </si>
+  <si>
     <t>thram_number</t>
   </si>
   <si>
@@ -70,28 +76,19 @@
   </si>
   <si>
     <t>dzongkhag</t>
-  </si>
-  <si>
-    <t>gurdian_contact</t>
-  </si>
-  <si>
-    <t>y-m-d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,27 +99,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -131,9 +113,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,32 +410,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" customWidth="1"/>
     <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" customWidth="1"/>
     <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="1025" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,56 +481,257 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" spans="1:26">
+      <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+    </row>
+    <row r="3" spans="1:26">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>